<commit_message>
get China country total OK
</commit_message>
<xml_diff>
--- a/RatingScore.xlsx
+++ b/RatingScore.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\risk_report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhangst\git\risk_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D56A8D-3FD5-4886-AB6F-6FAC23E2192E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D4F5EE-0EC2-41A1-B0A5-8FAF098B7784}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="81">
   <si>
     <t>S&amp;P</t>
   </si>
@@ -264,6 +264,18 @@
   </si>
   <si>
     <t>Agency</t>
+  </si>
+  <si>
+    <t>BBB *-</t>
+  </si>
+  <si>
+    <t>Added by Steven Zhang, needs to confirm with Daphne</t>
+  </si>
+  <si>
+    <t>Caa1u</t>
+  </si>
+  <si>
+    <t>B1u</t>
   </si>
 </sst>
 </file>
@@ -287,12 +299,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -307,9 +325,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,15 +609,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C99"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>76</v>
       </c>
@@ -609,7 +628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -620,7 +639,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -631,7 +650,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -642,7 +661,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -653,7 +672,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -664,7 +683,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -675,7 +694,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -686,7 +705,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -697,7 +716,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -708,7 +727,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -719,7 +738,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -730,7 +749,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -741,7 +760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -752,7 +771,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -763,7 +782,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -774,7 +793,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -785,7 +804,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -796,7 +815,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -807,7 +826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -818,7 +837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -829,7 +848,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -840,7 +859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -851,7 +870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -862,7 +881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -873,7 +892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -884,7 +903,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -895,7 +914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -906,7 +925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -917,7 +936,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -928,7 +947,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -939,7 +958,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -950,7 +969,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -961,7 +980,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -972,7 +991,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -983,7 +1002,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -994,7 +1013,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -1005,7 +1024,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -1016,7 +1035,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -1027,7 +1046,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -1038,7 +1057,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -1049,7 +1068,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -1060,7 +1079,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -1071,7 +1090,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -1082,610 +1101,663 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>2</v>
-      </c>
-      <c r="B45" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="2">
+        <v>8</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" t="s">
         <v>33</v>
       </c>
-      <c r="C45">
+      <c r="C46">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>2</v>
-      </c>
-      <c r="B46" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" t="s">
         <v>35</v>
       </c>
-      <c r="C46">
+      <c r="C47">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
         <v>37</v>
       </c>
-      <c r="C47">
+      <c r="C48">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>2</v>
-      </c>
-      <c r="B48" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C49" s="2">
+        <v>5</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G49" s="2"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
         <v>39</v>
       </c>
-      <c r="C48">
+      <c r="C50">
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>2</v>
-      </c>
-      <c r="B49" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
         <v>41</v>
       </c>
-      <c r="C49">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>2</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="C51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" t="s">
         <v>43</v>
       </c>
-      <c r="C50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>2</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="C52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" t="s">
         <v>44</v>
       </c>
-      <c r="C51">
+      <c r="C53">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>2</v>
-      </c>
-      <c r="B52" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" t="s">
         <v>46</v>
       </c>
-      <c r="C52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>2</v>
-      </c>
-      <c r="B53" t="s">
+      <c r="C54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" t="s">
         <v>48</v>
       </c>
-      <c r="C53">
+      <c r="C55">
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>2</v>
-      </c>
-      <c r="B54" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" t="s">
         <v>50</v>
       </c>
-      <c r="C54">
+      <c r="C56">
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>2</v>
-      </c>
-      <c r="B55" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" t="s">
         <v>52</v>
       </c>
-      <c r="C55">
+      <c r="C57">
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>2</v>
-      </c>
-      <c r="B56" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" t="s">
         <v>55</v>
       </c>
-      <c r="C56">
+      <c r="C58">
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>2</v>
-      </c>
-      <c r="B57" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" t="s">
         <v>57</v>
       </c>
-      <c r="C57">
+      <c r="C59">
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>2</v>
-      </c>
-      <c r="B58" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" t="s">
         <v>60</v>
       </c>
-      <c r="C58">
+      <c r="C60">
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>2</v>
-      </c>
-      <c r="B59" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" t="s">
         <v>63</v>
       </c>
-      <c r="C59">
+      <c r="C61">
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>2</v>
-      </c>
-      <c r="B60" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>2</v>
+      </c>
+      <c r="B62" t="s">
         <v>65</v>
       </c>
-      <c r="C60">
+      <c r="C62">
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>2</v>
-      </c>
-      <c r="B61" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" t="s">
         <v>67</v>
       </c>
-      <c r="C61">
+      <c r="C63">
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>3</v>
-      </c>
-      <c r="B62" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" t="s">
         <v>4</v>
       </c>
-      <c r="C62">
+      <c r="C64">
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>3</v>
-      </c>
-      <c r="B63" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" t="s">
         <v>6</v>
       </c>
-      <c r="C63">
+      <c r="C65">
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>3</v>
-      </c>
-      <c r="B64" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" t="s">
         <v>8</v>
       </c>
-      <c r="C64">
+      <c r="C66">
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>3</v>
-      </c>
-      <c r="B65" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67" t="s">
         <v>10</v>
       </c>
-      <c r="C65">
+      <c r="C67">
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>3</v>
-      </c>
-      <c r="B66" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68" t="s">
         <v>12</v>
       </c>
-      <c r="C66">
+      <c r="C68">
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>3</v>
-      </c>
-      <c r="B67" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" t="s">
         <v>14</v>
       </c>
-      <c r="C67">
+      <c r="C69">
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>3</v>
-      </c>
-      <c r="B68" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" t="s">
         <v>16</v>
       </c>
-      <c r="C68">
+      <c r="C70">
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>3</v>
-      </c>
-      <c r="B69" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71" t="s">
         <v>18</v>
       </c>
-      <c r="C69">
+      <c r="C71">
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>3</v>
-      </c>
-      <c r="B70" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72" t="s">
         <v>20</v>
       </c>
-      <c r="C70">
+      <c r="C72">
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>3</v>
-      </c>
-      <c r="B71" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73" t="s">
         <v>22</v>
       </c>
-      <c r="C71">
+      <c r="C73">
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>3</v>
-      </c>
-      <c r="B72" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74" t="s">
         <v>24</v>
       </c>
-      <c r="C72">
+      <c r="C74">
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>3</v>
-      </c>
-      <c r="B73" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75" t="s">
         <v>26</v>
       </c>
-      <c r="C73">
+      <c r="C75">
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>3</v>
-      </c>
-      <c r="B74" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76" t="s">
         <v>28</v>
       </c>
-      <c r="C74">
+      <c r="C76">
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>3</v>
-      </c>
-      <c r="B75" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77" t="s">
         <v>30</v>
       </c>
-      <c r="C75">
+      <c r="C77">
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>3</v>
-      </c>
-      <c r="B76" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" t="s">
         <v>32</v>
       </c>
-      <c r="C76">
+      <c r="C78">
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>3</v>
-      </c>
-      <c r="B77" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79" t="s">
         <v>34</v>
       </c>
-      <c r="C77">
+      <c r="C79">
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>3</v>
-      </c>
-      <c r="B78" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80" t="s">
         <v>36</v>
       </c>
-      <c r="C78">
+      <c r="C80">
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>3</v>
-      </c>
-      <c r="B79" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81" t="s">
         <v>38</v>
       </c>
-      <c r="C79">
+      <c r="C81">
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>3</v>
-      </c>
-      <c r="B80" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82" t="s">
         <v>40</v>
       </c>
-      <c r="C80">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>3</v>
-      </c>
-      <c r="B81" t="s">
+      <c r="C82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83" t="s">
         <v>42</v>
       </c>
-      <c r="C81">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>3</v>
-      </c>
-      <c r="B82" t="s">
+      <c r="C83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84" t="s">
         <v>44</v>
       </c>
-      <c r="C82">
+      <c r="C84">
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>3</v>
-      </c>
-      <c r="B83" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85" t="s">
         <v>45</v>
       </c>
-      <c r="C83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>3</v>
-      </c>
-      <c r="B84" t="s">
+      <c r="C85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86" t="s">
         <v>47</v>
       </c>
-      <c r="C84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>3</v>
-      </c>
-      <c r="B85" t="s">
+      <c r="C86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" t="s">
         <v>49</v>
       </c>
-      <c r="C85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>3</v>
-      </c>
-      <c r="B86" t="s">
+      <c r="C87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88" t="s">
         <v>53</v>
       </c>
-      <c r="C86">
+      <c r="C88">
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>3</v>
-      </c>
-      <c r="B87" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>3</v>
+      </c>
+      <c r="B89" t="s">
         <v>51</v>
       </c>
-      <c r="C87">
+      <c r="C89">
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>3</v>
-      </c>
-      <c r="B88" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90" t="s">
         <v>58</v>
       </c>
-      <c r="C88">
+      <c r="C90">
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>3</v>
-      </c>
-      <c r="B89" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91" t="s">
         <v>61</v>
       </c>
-      <c r="C89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>3</v>
-      </c>
-      <c r="B90" t="s">
+      <c r="C91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>3</v>
+      </c>
+      <c r="B92" t="s">
         <v>64</v>
       </c>
-      <c r="C90">
+      <c r="C92">
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>3</v>
-      </c>
-      <c r="B91" t="s">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>3</v>
+      </c>
+      <c r="B93" t="s">
         <v>66</v>
       </c>
-      <c r="C91">
+      <c r="C93">
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>3</v>
-      </c>
-      <c r="B92" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>3</v>
+      </c>
+      <c r="B94" t="s">
         <v>68</v>
       </c>
-      <c r="C92">
+      <c r="C94">
         <v>21</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>3</v>
-      </c>
-      <c r="B93" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>3</v>
+      </c>
+      <c r="B95" t="s">
         <v>69</v>
       </c>
-      <c r="C93">
+      <c r="C95">
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>3</v>
-      </c>
-      <c r="B94" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>3</v>
+      </c>
+      <c r="B96" t="s">
         <v>70</v>
       </c>
-      <c r="C94">
+      <c r="C96">
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>3</v>
-      </c>
-      <c r="B95" t="s">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>3</v>
+      </c>
+      <c r="B97" t="s">
         <v>56</v>
-      </c>
-      <c r="C95">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>3</v>
-      </c>
-      <c r="B96" t="s">
-        <v>71</v>
-      </c>
-      <c r="C96">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>3</v>
-      </c>
-      <c r="B97" t="s">
-        <v>72</v>
       </c>
       <c r="C97">
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>3</v>
       </c>
       <c r="B98" t="s">
+        <v>71</v>
+      </c>
+      <c r="C98">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>3</v>
+      </c>
+      <c r="B99" t="s">
+        <v>72</v>
+      </c>
+      <c r="C99">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>3</v>
+      </c>
+      <c r="B100" t="s">
         <v>73</v>
       </c>
-      <c r="C98">
+      <c r="C100">
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>3</v>
-      </c>
-      <c r="B99" t="s">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>3</v>
+      </c>
+      <c r="B101" t="s">
         <v>74</v>
       </c>
-      <c r="C99">
+      <c r="C101">
         <v>7</v>
       </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C102" s="2">
+        <v>13</v>
+      </c>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G102" s="2"/>
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
refactored code, using utils.excel package instead of clamc_datafeed.feeder package
</commit_message>
<xml_diff>
--- a/RatingScore.xlsx
+++ b/RatingScore.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhangst\git\risk_report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\risk_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D4F5EE-0EC2-41A1-B0A5-8FAF098B7784}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA997649-D8F8-441F-B95B-D839C4461FF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31890" yWindow="390" windowWidth="21960" windowHeight="14850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="82">
   <si>
     <t>S&amp;P</t>
   </si>
@@ -269,13 +269,16 @@
     <t>BBB *-</t>
   </si>
   <si>
-    <t>Added by Steven Zhang, needs to confirm with Daphne</t>
-  </si>
-  <si>
     <t>Caa1u</t>
   </si>
   <si>
     <t>B1u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In recent years, Moody’s added “u”  or “e” identifier to express additional meanings on their ratings. These identifiers do not change the associated rating score actually. </t>
+  </si>
+  <si>
+    <t>Same as "BBB"</t>
   </si>
 </sst>
 </file>
@@ -299,18 +302,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -328,7 +325,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,15 +606,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>76</v>
       </c>
@@ -628,7 +625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -639,7 +636,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -650,7 +647,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -661,7 +658,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -672,7 +669,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -683,7 +680,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -694,7 +691,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -705,7 +702,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -716,7 +713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -727,7 +724,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -738,7 +735,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -749,7 +746,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -760,7 +757,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -771,7 +768,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -782,7 +779,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -793,7 +790,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -804,7 +801,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -815,7 +812,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -826,7 +823,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -837,7 +834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -848,7 +845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -859,7 +856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -870,7 +867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -881,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -892,7 +889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -903,7 +900,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -914,7 +911,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -925,7 +922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -936,7 +933,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -947,7 +944,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -958,7 +955,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -969,7 +966,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -980,7 +977,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -991,7 +988,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -1002,7 +999,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -1013,7 +1010,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -1024,7 +1021,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -1035,7 +1032,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -1046,7 +1043,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -1057,7 +1054,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -1068,7 +1065,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -1079,7 +1076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -1090,7 +1087,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -1101,12 +1098,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C45" s="2">
         <v>8</v>
@@ -1114,11 +1111,11 @@
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -1129,7 +1126,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -1140,7 +1137,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>2</v>
       </c>
@@ -1151,24 +1148,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C49" s="2">
         <v>5</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
-      <c r="F49" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="F49" s="2"/>
       <c r="G49" s="2"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -1179,7 +1174,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>2</v>
       </c>
@@ -1190,7 +1185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -1201,7 +1196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>2</v>
       </c>
@@ -1212,7 +1207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>2</v>
       </c>
@@ -1223,7 +1218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -1234,7 +1229,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -1245,7 +1240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -1256,7 +1251,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -1267,7 +1262,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>2</v>
       </c>
@@ -1278,7 +1273,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>2</v>
       </c>
@@ -1289,7 +1284,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>2</v>
       </c>
@@ -1300,7 +1295,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>2</v>
       </c>
@@ -1311,7 +1306,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>2</v>
       </c>
@@ -1322,7 +1317,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>3</v>
       </c>
@@ -1333,7 +1328,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>3</v>
       </c>
@@ -1344,7 +1339,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>3</v>
       </c>
@@ -1355,7 +1350,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -1366,7 +1361,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>3</v>
       </c>
@@ -1377,7 +1372,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>3</v>
       </c>
@@ -1388,7 +1383,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>3</v>
       </c>
@@ -1399,7 +1394,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>3</v>
       </c>
@@ -1410,7 +1405,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>3</v>
       </c>
@@ -1421,343 +1416,346 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>3</v>
-      </c>
-      <c r="B73" t="s">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C73" s="2">
+        <v>13</v>
+      </c>
+      <c r="F73" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74" t="s">
         <v>22</v>
       </c>
-      <c r="C73">
+      <c r="C74">
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>3</v>
-      </c>
-      <c r="B74" t="s">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75" t="s">
         <v>24</v>
       </c>
-      <c r="C74">
+      <c r="C75">
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>3</v>
-      </c>
-      <c r="B75" t="s">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76" t="s">
         <v>26</v>
       </c>
-      <c r="C75">
+      <c r="C76">
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>3</v>
-      </c>
-      <c r="B76" t="s">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77" t="s">
         <v>28</v>
       </c>
-      <c r="C76">
+      <c r="C77">
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>3</v>
-      </c>
-      <c r="B77" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" t="s">
         <v>30</v>
       </c>
-      <c r="C77">
+      <c r="C78">
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>3</v>
-      </c>
-      <c r="B78" t="s">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79" t="s">
         <v>32</v>
       </c>
-      <c r="C78">
+      <c r="C79">
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>3</v>
-      </c>
-      <c r="B79" t="s">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80" t="s">
         <v>34</v>
       </c>
-      <c r="C79">
+      <c r="C80">
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>3</v>
-      </c>
-      <c r="B80" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81" t="s">
         <v>36</v>
       </c>
-      <c r="C80">
+      <c r="C81">
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>3</v>
-      </c>
-      <c r="B81" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82" t="s">
         <v>38</v>
       </c>
-      <c r="C81">
+      <c r="C82">
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>3</v>
-      </c>
-      <c r="B82" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83" t="s">
         <v>40</v>
       </c>
-      <c r="C82">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>3</v>
-      </c>
-      <c r="B83" t="s">
+      <c r="C83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84" t="s">
         <v>42</v>
       </c>
-      <c r="C83">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>3</v>
-      </c>
-      <c r="B84" t="s">
+      <c r="C84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85" t="s">
         <v>44</v>
       </c>
-      <c r="C84">
+      <c r="C85">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>3</v>
-      </c>
-      <c r="B85" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86" t="s">
         <v>45</v>
       </c>
-      <c r="C85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>3</v>
-      </c>
-      <c r="B86" t="s">
+      <c r="C86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" t="s">
         <v>47</v>
       </c>
-      <c r="C86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>3</v>
-      </c>
-      <c r="B87" t="s">
+      <c r="C87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88" t="s">
         <v>49</v>
       </c>
-      <c r="C87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>3</v>
-      </c>
-      <c r="B88" t="s">
+      <c r="C88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>3</v>
+      </c>
+      <c r="B89" t="s">
         <v>53</v>
-      </c>
-      <c r="C88">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>3</v>
-      </c>
-      <c r="B89" t="s">
-        <v>51</v>
       </c>
       <c r="C89">
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>3</v>
       </c>
       <c r="B90" t="s">
+        <v>51</v>
+      </c>
+      <c r="C90">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91" t="s">
         <v>58</v>
       </c>
-      <c r="C90">
+      <c r="C91">
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>3</v>
-      </c>
-      <c r="B91" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>3</v>
+      </c>
+      <c r="B92" t="s">
         <v>61</v>
       </c>
-      <c r="C91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>3</v>
-      </c>
-      <c r="B92" t="s">
+      <c r="C92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>3</v>
+      </c>
+      <c r="B93" t="s">
         <v>64</v>
       </c>
-      <c r="C92">
+      <c r="C93">
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>3</v>
-      </c>
-      <c r="B93" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>3</v>
+      </c>
+      <c r="B94" t="s">
         <v>66</v>
       </c>
-      <c r="C93">
+      <c r="C94">
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>3</v>
-      </c>
-      <c r="B94" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>3</v>
+      </c>
+      <c r="B95" t="s">
         <v>68</v>
       </c>
-      <c r="C94">
+      <c r="C95">
         <v>21</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>3</v>
-      </c>
-      <c r="B95" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>3</v>
+      </c>
+      <c r="B96" t="s">
         <v>69</v>
       </c>
-      <c r="C95">
+      <c r="C96">
         <v>13</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>3</v>
-      </c>
-      <c r="B96" t="s">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>3</v>
+      </c>
+      <c r="B97" t="s">
         <v>70</v>
       </c>
-      <c r="C96">
+      <c r="C97">
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>3</v>
-      </c>
-      <c r="B97" t="s">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>3</v>
+      </c>
+      <c r="B98" t="s">
         <v>56</v>
-      </c>
-      <c r="C97">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>3</v>
-      </c>
-      <c r="B98" t="s">
-        <v>71</v>
       </c>
       <c r="C98">
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>3</v>
       </c>
       <c r="B99" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C99">
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>3</v>
       </c>
       <c r="B100" t="s">
+        <v>72</v>
+      </c>
+      <c r="C100">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>3</v>
+      </c>
+      <c r="B101" t="s">
         <v>73</v>
       </c>
-      <c r="C100">
+      <c r="C101">
         <v>14</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>3</v>
-      </c>
-      <c r="B101" t="s">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>3</v>
+      </c>
+      <c r="B102" t="s">
         <v>74</v>
       </c>
-      <c r="C101">
+      <c r="C102">
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A102" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C102" s="2">
-        <v>13</v>
-      </c>
-      <c r="D102" s="2"/>
-      <c r="E102" s="2"/>
-      <c r="F102" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
-      <c r="I102" s="2"/>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
+      <c r="I103" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated liquidity logic, added liquidity override. but now the result differ as of 2020-06-30
</commit_message>
<xml_diff>
--- a/RatingScore.xlsx
+++ b/RatingScore.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\risk_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A6455B-BA51-4179-BBCD-3E42E5092195}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B2514F-E1A3-437E-A1FC-63F8790F6F1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="100">
   <si>
     <t>S&amp;P</t>
   </si>
@@ -278,12 +278,21 @@
     <t xml:space="preserve">In recent years, Moody’s added “u”  or “e” identifier to express additional meanings on their ratings. These identifiers do not change the associated rating score actually. </t>
   </si>
   <si>
+    <t>Same as "BBB"</t>
+  </si>
+  <si>
     <t>BBBu</t>
   </si>
   <si>
     <t>Au</t>
   </si>
   <si>
+    <t>Same as "A"</t>
+  </si>
+  <si>
+    <t>Guessed by Steven, to be confirmed</t>
+  </si>
+  <si>
     <t>F1+</t>
   </si>
   <si>
@@ -324,9 +333,6 @@
   </si>
   <si>
     <t>B3 *-</t>
-  </si>
-  <si>
-    <t>B- *</t>
   </si>
 </sst>
 </file>
@@ -661,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,10 +691,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -696,10 +702,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -707,10 +713,10 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -718,10 +724,10 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -729,22 +735,24 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>95</v>
       </c>
       <c r="C6">
         <v>18</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -752,10 +760,10 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C8">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -763,10 +771,10 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -774,10 +782,10 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="C10">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -785,10 +793,10 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C11">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -796,10 +804,10 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C12">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -807,10 +815,10 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -818,10 +826,10 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="C14">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -829,10 +837,10 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -840,10 +848,10 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C16">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -851,10 +859,10 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C17">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -862,10 +870,10 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="C18">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -873,10 +881,10 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C19">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -884,10 +892,10 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C20">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -895,10 +903,10 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C21">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -906,10 +914,10 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C22">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -917,10 +925,10 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C23">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -928,10 +936,10 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C24">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -939,10 +947,10 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="C25">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -950,10 +958,10 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -961,10 +969,10 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -972,10 +980,10 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C28">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -983,10 +991,10 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="C29">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -994,10 +1002,10 @@
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C30">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1005,32 +1013,32 @@
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1038,10 +1046,10 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C34">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1049,10 +1057,10 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="C35">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1060,10 +1068,10 @@
         <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="C36">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1071,18 +1079,21 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="C37">
         <v>17</v>
       </c>
+      <c r="F37" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C38">
         <v>17</v>
@@ -1093,22 +1104,21 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="C39">
-        <v>17</v>
-      </c>
-      <c r="F39" s="3"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>2</v>
       </c>
       <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40">
         <v>15</v>
-      </c>
-      <c r="C40">
-        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1116,7 +1126,7 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="C41">
         <v>15</v>
@@ -1127,21 +1137,24 @@
         <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C42">
         <v>15</v>
       </c>
+      <c r="F42" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>19</v>
       </c>
       <c r="C43">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1149,22 +1162,21 @@
         <v>2</v>
       </c>
       <c r="B44" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C44">
-        <v>20</v>
-      </c>
-      <c r="F44" s="3"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C45">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1172,10 +1184,10 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46">
         <v>11</v>
-      </c>
-      <c r="C46">
-        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1183,10 +1195,10 @@
         <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C47">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1194,10 +1206,10 @@
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="C48">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -1205,10 +1217,10 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="C49">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1221,6 +1233,12 @@
       <c r="C50" s="2">
         <v>8</v>
       </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G50" s="2"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -1238,24 +1256,18 @@
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="C52">
-        <v>7</v>
-      </c>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G52" s="2"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="C53">
         <v>6</v>
@@ -1266,32 +1278,36 @@
         <v>2</v>
       </c>
       <c r="B54" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
       <c r="C54">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>2</v>
-      </c>
-      <c r="B55" t="s">
-        <v>25</v>
-      </c>
-      <c r="C55">
-        <v>11</v>
-      </c>
+      <c r="A55" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="2">
+        <v>5</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>2</v>
       </c>
       <c r="B56" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C56">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -1299,25 +1315,21 @@
         <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C57">
-        <v>10</v>
-      </c>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>2</v>
       </c>
       <c r="B58" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="C58">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -1325,10 +1337,10 @@
         <v>2</v>
       </c>
       <c r="B59" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C59">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -1336,10 +1348,10 @@
         <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C60">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -1347,10 +1359,10 @@
         <v>2</v>
       </c>
       <c r="B61" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C61">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -1358,10 +1370,10 @@
         <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="C62">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -1369,7 +1381,7 @@
         <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="C63">
         <v>12</v>
@@ -1380,10 +1392,10 @@
         <v>2</v>
       </c>
       <c r="B64" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C64">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1391,10 +1403,10 @@
         <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1402,10 +1414,10 @@
         <v>2</v>
       </c>
       <c r="B66" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C66">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1413,21 +1425,21 @@
         <v>2</v>
       </c>
       <c r="B67" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="C67">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C68" s="2">
-        <v>5</v>
+      <c r="A68" t="s">
+        <v>2</v>
+      </c>
+      <c r="B68" t="s">
+        <v>65</v>
+      </c>
+      <c r="C68">
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1435,10 +1447,10 @@
         <v>2</v>
       </c>
       <c r="B69" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="C69">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1446,44 +1458,46 @@
         <v>2</v>
       </c>
       <c r="B70" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C70">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B71" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B72" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="C72">
-        <v>0</v>
-      </c>
-      <c r="F72" s="3"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>3</v>
       </c>
       <c r="B73" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C73">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -1491,10 +1505,10 @@
         <v>3</v>
       </c>
       <c r="B74" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C74">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -1502,10 +1516,10 @@
         <v>3</v>
       </c>
       <c r="B75" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C75">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -1513,10 +1527,10 @@
         <v>3</v>
       </c>
       <c r="B76" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="C76">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -1524,10 +1538,13 @@
         <v>3</v>
       </c>
       <c r="B77" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C77">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="F77" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -1535,10 +1552,10 @@
         <v>3</v>
       </c>
       <c r="B78" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C78">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -1546,10 +1563,10 @@
         <v>3</v>
       </c>
       <c r="B79" t="s">
-        <v>86</v>
+        <v>18</v>
       </c>
       <c r="C79">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -1557,10 +1574,10 @@
         <v>3</v>
       </c>
       <c r="B80" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C80">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -1568,10 +1585,10 @@
         <v>3</v>
       </c>
       <c r="B81" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C81">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -1579,21 +1596,27 @@
         <v>3</v>
       </c>
       <c r="B82" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="C82">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="F82" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>3</v>
-      </c>
-      <c r="B83" t="s">
-        <v>6</v>
-      </c>
-      <c r="C83">
-        <v>20</v>
+      <c r="A83" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C83" s="2">
+        <v>13</v>
+      </c>
+      <c r="F83" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -1601,10 +1624,10 @@
         <v>3</v>
       </c>
       <c r="B84" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="C84">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -1612,10 +1635,13 @@
         <v>3</v>
       </c>
       <c r="B85" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="C85">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -1623,10 +1649,10 @@
         <v>3</v>
       </c>
       <c r="B86" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="C86">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -1634,22 +1660,21 @@
         <v>3</v>
       </c>
       <c r="B87" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="C87">
-        <v>15</v>
-      </c>
-      <c r="F87" s="3"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>3</v>
       </c>
       <c r="B88" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C88">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -1657,10 +1682,10 @@
         <v>3</v>
       </c>
       <c r="B89" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C89">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -1668,10 +1693,10 @@
         <v>3</v>
       </c>
       <c r="B90" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="C90">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -1679,10 +1704,10 @@
         <v>3</v>
       </c>
       <c r="B91" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C91">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -1690,10 +1715,10 @@
         <v>3</v>
       </c>
       <c r="B92" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="C92">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -1701,10 +1726,10 @@
         <v>3</v>
       </c>
       <c r="B93" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C93">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -1712,10 +1737,10 @@
         <v>3</v>
       </c>
       <c r="B94" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C94">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -1723,10 +1748,10 @@
         <v>3</v>
       </c>
       <c r="B95" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C95">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -1734,10 +1759,10 @@
         <v>3</v>
       </c>
       <c r="B96" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C96">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -1745,10 +1770,10 @@
         <v>3</v>
       </c>
       <c r="B97" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="C97">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -1756,10 +1781,10 @@
         <v>3</v>
       </c>
       <c r="B98" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C98">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -1767,21 +1792,24 @@
         <v>3</v>
       </c>
       <c r="B99" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="C99">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C100" s="2">
-        <v>12</v>
+      <c r="A100" t="s">
+        <v>3</v>
+      </c>
+      <c r="B100" t="s">
+        <v>93</v>
+      </c>
+      <c r="C100">
+        <v>17</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -1789,35 +1817,46 @@
         <v>3</v>
       </c>
       <c r="B101" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="C101">
-        <v>14</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F101" s="3"/>
+      <c r="G101" s="3"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>3</v>
       </c>
       <c r="B102" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="C102">
-        <v>14</v>
-      </c>
-      <c r="E102" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>3</v>
       </c>
       <c r="B103" t="s">
+        <v>90</v>
+      </c>
+      <c r="C103">
+        <v>15</v>
+      </c>
+      <c r="E103" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C103">
-        <v>14</v>
-      </c>
-      <c r="E103" s="3"/>
       <c r="F103" s="3"/>
       <c r="G103" s="3"/>
     </row>
@@ -1826,38 +1865,32 @@
         <v>3</v>
       </c>
       <c r="B104" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C104">
-        <v>13</v>
-      </c>
-      <c r="E104" s="3"/>
-      <c r="F104" s="3"/>
-      <c r="G104" s="3"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>3</v>
       </c>
       <c r="B105" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C105">
-        <v>12</v>
-      </c>
-      <c r="E105" s="3"/>
-      <c r="F105" s="3"/>
-      <c r="G105" s="3"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>3</v>
       </c>
       <c r="B106" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="C106">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -1865,10 +1898,10 @@
         <v>3</v>
       </c>
       <c r="B107" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C107">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -1876,10 +1909,10 @@
         <v>3</v>
       </c>
       <c r="B108" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C108">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -1887,10 +1920,10 @@
         <v>3</v>
       </c>
       <c r="B109" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C109">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -1898,10 +1931,10 @@
         <v>3</v>
       </c>
       <c r="B110" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C110">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -1909,10 +1942,10 @@
         <v>3</v>
       </c>
       <c r="B111" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="C111">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -1920,10 +1953,10 @@
         <v>3</v>
       </c>
       <c r="B112" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="C112">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -1931,10 +1964,10 @@
         <v>3</v>
       </c>
       <c r="B113" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C113">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -1942,10 +1975,10 @@
         <v>3</v>
       </c>
       <c r="B114" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="C114">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -1953,10 +1986,10 @@
         <v>3</v>
       </c>
       <c r="B115" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C115">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -1964,10 +1997,10 @@
         <v>3</v>
       </c>
       <c r="B116" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="C116">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -1975,10 +2008,10 @@
         <v>3</v>
       </c>
       <c r="B117" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -1986,58 +2019,37 @@
         <v>3</v>
       </c>
       <c r="B118" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C118">
         <v>0</v>
       </c>
+      <c r="D118" s="2"/>
+      <c r="E118" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F118" s="3"/>
+      <c r="G118" s="3"/>
+      <c r="H118" s="2"/>
+      <c r="I118" s="2"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>3</v>
       </c>
       <c r="B119" t="s">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="C119">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>3</v>
-      </c>
-      <c r="B120" t="s">
-        <v>47</v>
-      </c>
-      <c r="C120">
-        <v>0</v>
-      </c>
-      <c r="D120" s="2"/>
-      <c r="E120" s="3"/>
-      <c r="F120" s="3"/>
-      <c r="G120" s="3"/>
-      <c r="H120" s="2"/>
-      <c r="I120" s="2"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>3</v>
-      </c>
-      <c r="B121" t="s">
-        <v>61</v>
-      </c>
-      <c r="C121">
-        <v>0</v>
-      </c>
-      <c r="E121" s="3"/>
-      <c r="F121" s="3"/>
-      <c r="G121" s="3"/>
+      <c r="E119" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F119" s="3"/>
+      <c r="G119" s="3"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A74:C121">
-    <sortCondition ref="B74:B121"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>